<commit_message>
COC number not required
</commit_message>
<xml_diff>
--- a/FSK_LowFlow definition.xlsx
+++ b/FSK_LowFlow definition.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="10335" tabRatio="537" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="10335" tabRatio="537" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Format Information" sheetId="1" r:id="rId1"/>
     <sheet name="FieldSampleKey" sheetId="2" r:id="rId2"/>
     <sheet name="LowFlowSampling" sheetId="3" r:id="rId3"/>
+    <sheet name="Error Checks" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>#project_number</t>
   </si>
@@ -312,6 +313,480 @@
   </si>
   <si>
     <t>Note: Red means required</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>ml/min</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>gal</t>
+  </si>
+  <si>
+    <t>l/min</t>
+  </si>
+  <si>
+    <t>gal/min</t>
+  </si>
+  <si>
+    <t>Deg C</t>
+  </si>
+  <si>
+    <t>Deg F</t>
+  </si>
+  <si>
+    <t>ph Units</t>
+  </si>
+  <si>
+    <t>mS/cm</t>
+  </si>
+  <si>
+    <t>uS/cm</t>
+  </si>
+  <si>
+    <t>PSS</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>mv</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Percent_moisture cannot be null when sample matrix = SO or SE and sample type = N, FD, FR, FS, LR, MS, SD or MSD. (1)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Reportable_result cannot be 'Yes' where lab_qualifiers=E, G, P, or R. (2)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Datum_unit cannot be null if datum_value is not null. (3)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Sample must have related test/result. (20)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Reporting_detection_limit cannot be null when detect_flag=N. (5)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Result_value is required where detect_flag=Y and result_type_code=TRG, TIC. (6)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Cannot be less than the original concentration. (7)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Subsample_amount and subsample_amount_unit cannot be null when sample type = N, FD, FR, FS, LR, MS, SD or MSD. (8)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Date cannot precede sample_date. (9)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Parent_sample_code is required where sample_type_code= " &amp; customError10Message &amp; " (10)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Sample_date cannot be null when when sample_type_code=TB, N, MB, FD, FB, EB, AB. (11)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>12.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Start_depth cannot be null when sample_matrix_code=SO or SE. (12)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>13.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"If start_depth is not null, end_depth must be greater than start_depth. (13)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>14.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Lab_name_code cannot be null when analysis_location=LB or FL. (14)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>15.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Lab_sample_id cannot be null when analysis_location=LB. (15)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>16.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Result_unit cannot be null when result_value is not null. (16)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>17.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Detection_limit_unit cannot be null when reporting_detection_limit is not null. (17)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>18.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Depth_unit cannot be null if start_depth is not null. (18)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>19.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Sample_time cannot be null when sample_type_code=TB, N, MB, FD, FB, EB, AB. (19)"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>20.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"If analysis_location=LB, sample_delivery_group, sent_to_lab_date, and sample_receipt_date cannot be null. (20)"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -323,7 +798,7 @@
     <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
@@ -364,8 +839,18 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +881,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -409,7 +900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -422,6 +913,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -894,7 +1389,7 @@
       <c r="W1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" t="s">
         <v>34</v>
       </c>
       <c r="Y1" t="s">
@@ -1043,11 +1538,11 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
     </row>
@@ -1437,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1692,28 +2187,114 @@
         <v>76</v>
       </c>
       <c r="C4" s="7"/>
+      <c r="Q4" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="7"/>
+      <c r="Q5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
     </row>
     <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="7"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
     </row>
     <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="7"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
     </row>
     <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:28" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="7"/>
@@ -1993,5 +2574,122 @@
     <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>